<commit_message>
Put data together in gui class
</commit_message>
<xml_diff>
--- a/data/referrals/referrals.xlsx
+++ b/data/referrals/referrals.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$6</definedName>
-    <definedName name="referrals" localSheetId="0">Sheet1!$A$1:$G$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$7</definedName>
+    <definedName name="referrals" localSheetId="0">Sheet1!$A$1:$H$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,9 +29,10 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="referrals" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="65001" sourceFile="J:\ARPS\data\referrals\referrals.txt">
-      <textFields count="7">
+  <connection id="1" name="referrals" type="6" refreshedVersion="5" background="1" refreshOnLoad="1" saveData="1">
+    <textPr prompt="0" codePage="65001" sourceFile="J:\ARPS\data\referrals\referrals.txt">
+      <textFields count="8">
+        <textField/>
         <textField/>
         <textField type="text"/>
         <textField/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>SENDER_NUMBER</t>
   </si>
@@ -160,6 +161,27 @@
   </si>
   <si>
     <t>Hismomisareallyactivemember.Heisanlabuthiswifeisbuddhist.Worksasanaccountantandhas3kids.Hismomsaysthatheisareallywellbehavedboyanddeepdownlovesthegospel.Atonepointwantedtogoonamission.Howeverdoesntgotochurchbecauseofthewife.Willingtohavethemissionariesover!Himandhisfamilyliveonbaoqiaolu78shang20hao17nong.</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>2016:2:4:7</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>田凹凸</t>
+  </si>
+  <si>
+    <t>一個測試</t>
+  </si>
+  <si>
+    <t>+886910358944</t>
+  </si>
+  <si>
+    <t>0987017211</t>
   </si>
 </sst>
 </file>
@@ -217,7 +239,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="referrals" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="referrals" refreshOnLoad="1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,160 +505,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:8">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8">
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G6"/>
+  <autoFilter ref="A1:H7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>